<commit_message>
cleaned up formatting errors
</commit_message>
<xml_diff>
--- a/posts/primary/primary.xlsx
+++ b/posts/primary/primary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/n_moopen_uu_nl/Documents/Documents/programming/doy-data-inventory/posts/primary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="11_AD4DB114E441178AC67DF4D4FE17F604683EDF25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73BAE4D7-0280-4657-B706-5E2F060D02F0}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="11_AD4DB114E441178AC67DF4D4FE17F604683EDF25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3CFCB7C-1A43-4835-829D-BDC036B0D122}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -204,11 +204,6 @@
     <t>**Type of Research Instrument**</t>
   </si>
   <si>
-    <t>Aleva, A., van den Berg, T., Laceulle, O.M. et al. A smartphone-based intervention for young
-people who self-harm (‘PRIMARY’): study protocol for a multicenter randomized controlled trial.
-BMC Psychiatry 23, 840 (2023). doi: &lt;https://doi.org/10.1186/s12888-023-05301-x&gt;</t>
-  </si>
-  <si>
     <t>Christel Hessels (GGZ Centraal) - [ORCID](https://orcid.org/0000-0002-1937-1085)</t>
   </si>
   <si>
@@ -225,6 +220,9 @@
   </si>
   <si>
     <t>[Christel Hessels](c.hessels@ggzcentraal.nl) (GGZ Centraal)</t>
+  </si>
+  <si>
+    <t>Aleva, A., van den Berg, T., Laceulle, O.M. et al. A smartphone-based intervention for young people who self-harm (‘PRIMARY’): study protocol for a multicenter randomized controlled trial. BMC Psychiatry 23, 840 (2023). doi: &lt;https://doi.org/10.1186/s12888-023-05301-x&gt;</t>
   </si>
 </sst>
 </file>
@@ -316,10 +314,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,29 +581,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:A39"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -617,7 +611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -625,7 +619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>34</v>
       </c>
@@ -633,53 +627,53 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="11"/>
       <c r="B7" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="11"/>
       <c r="B8" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
       <c r="B9" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
       <c r="B10" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -687,7 +681,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -695,7 +689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
@@ -703,45 +697,45 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="11"/>
       <c r="B16" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="11"/>
       <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
       <c r="B18" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="11"/>
       <c r="B19" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="11"/>
       <c r="B20" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>41</v>
       </c>
@@ -749,7 +743,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>42</v>
       </c>
@@ -757,7 +751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>45</v>
       </c>
@@ -765,7 +759,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>43</v>
       </c>
@@ -773,7 +767,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>44</v>
       </c>
@@ -781,7 +775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>46</v>
       </c>
@@ -789,7 +783,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -797,7 +791,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
@@ -805,7 +799,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>49</v>
       </c>
@@ -813,7 +807,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>50</v>
       </c>
@@ -821,7 +815,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>51</v>
       </c>
@@ -829,13 +823,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>53</v>
       </c>
@@ -843,7 +837,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
         <v>54</v>
       </c>
@@ -851,7 +845,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>55</v>
       </c>
@@ -859,7 +853,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>56</v>
       </c>
@@ -867,7 +861,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>57</v>
       </c>
@@ -875,7 +869,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>58</v>
       </c>
@@ -883,7 +877,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -891,20 +885,20 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
     </row>
   </sheetData>

</xml_diff>